<commit_message>
Migration feature xpath updated
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp.xlsx
+++ b/Selenium-Scripts/src/DigitalApp.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="3" r:id="rId2"/>
-    <sheet name="HelpAndSupportPage" sheetId="4" r:id="rId3"/>
-    <sheet name="HomeMovePage" sheetId="7" r:id="rId4"/>
-    <sheet name="FeedBackPage" sheetId="6" r:id="rId5"/>
+    <sheet name="MigrationPage" sheetId="8" r:id="rId3"/>
+    <sheet name="HelpAndSupportPage" sheetId="4" r:id="rId4"/>
+    <sheet name="HomeMovePage" sheetId="7" r:id="rId5"/>
+    <sheet name="FeedBackPage" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Key</t>
   </si>
@@ -95,6 +96,12 @@
   </si>
   <si>
     <t>DigitalApp_Android_Identifiers</t>
+  </si>
+  <si>
+    <t>MigrationUsername</t>
+  </si>
+  <si>
+    <t>MigrationPassword</t>
   </si>
 </sst>
 </file>
@@ -495,19 +502,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -540,19 +547,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -560,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -568,7 +575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -576,7 +583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -584,11 +591,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -598,20 +621,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -619,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -627,7 +677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -635,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -649,7 +699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -657,13 +707,13 @@
       <selection activeCell="I27" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -671,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -679,7 +729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -692,7 +742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -700,13 +750,13 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -714,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -722,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Plans and Addons xpath update
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp.xlsx
+++ b/Selenium-Scripts/src/DigitalApp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Key</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>MigrationPassword</t>
+  </si>
+  <si>
+    <t>PlansAndAddonsUsername</t>
+  </si>
+  <si>
+    <t>PlansAndAddonsPassword</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,15 +553,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -615,6 +621,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -624,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Home Mome and other code level changes on Report
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp.xlsx
+++ b/Selenium-Scripts/src/DigitalApp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0A2E94-6B0F-E144-81E1-C0728C19CF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C4FC18-A9BB-A445-B53F-03762DBF119E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="2920" windowWidth="23040" windowHeight="9200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="HomeMovePage" sheetId="7" r:id="rId5"/>
     <sheet name="FeedBackPage" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Key</t>
   </si>
@@ -87,9 +87,6 @@
     <t>addressOnMap</t>
   </si>
   <si>
-    <t>World Trade Center</t>
-  </si>
-  <si>
     <t>FloorApartmentVilla</t>
   </si>
   <si>
@@ -103,13 +100,73 @@
   </si>
   <si>
     <t>DigitalApp_IOS_Identifiers</t>
+  </si>
+  <si>
+    <t>World Trade Center Mall</t>
+  </si>
+  <si>
+    <t>TelephoneNumber</t>
+  </si>
+  <si>
+    <t>092229774</t>
+  </si>
+  <si>
+    <t>The Dubai Mall</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>157.50</t>
+  </si>
+  <si>
+    <t>Account Number: 042545064</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>Packagename</t>
+  </si>
+  <si>
+    <t>eLife Unlimited Premium 500</t>
+  </si>
+  <si>
+    <t>InstallationAdress</t>
+  </si>
+  <si>
+    <t>DUBAI MALL 405 DX</t>
+  </si>
+  <si>
+    <t>Move-out date: Thu, 25 Mar 2021</t>
+  </si>
+  <si>
+    <t>Moveoutdate</t>
+  </si>
+  <si>
+    <t>05 439 34875</t>
+  </si>
+  <si>
+    <t>Yourcontactdetails</t>
+  </si>
+  <si>
+    <t>Installationdate</t>
+  </si>
+  <si>
+    <t>Fri, 26 Mar 2021, 8:00 am-12:00 pm</t>
+  </si>
+  <si>
+    <t>the world trade center abu dhabi</t>
+  </si>
+  <si>
+    <t>addressOutside</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +215,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -200,12 +278,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -503,11 +587,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
@@ -515,7 +599,7 @@
     <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,12 +613,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -551,16 +635,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -576,7 +660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -584,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -592,7 +676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -600,17 +684,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -629,13 +713,13 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -653,16 +737,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -670,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -678,7 +762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -686,7 +770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -702,19 +786,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -722,20 +806,92 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>22</v>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19">
+      <c r="A8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -745,19 +901,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -765,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -773,12 +929,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with Post Enhancement CRs
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp.xlsx
+++ b/Selenium-Scripts/src/DigitalApp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9192" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="HelpAndSupportPage" sheetId="4" r:id="rId4"/>
     <sheet name="HomeMovePage" sheetId="7" r:id="rId5"/>
     <sheet name="PlansAndAddonsPage" sheetId="10" r:id="rId6"/>
-    <sheet name="RechargeHistoryPage" sheetId="9" r:id="rId7"/>
-    <sheet name="FeedBackPage" sheetId="6" r:id="rId8"/>
+    <sheet name="PostEnhancement" sheetId="11" r:id="rId7"/>
+    <sheet name="RechargeHistoryPage" sheetId="9" r:id="rId8"/>
+    <sheet name="FeedBackPage" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>Key</t>
   </si>
@@ -269,13 +270,37 @@
   </si>
   <si>
     <t>Cancel subscription</t>
+  </si>
+  <si>
+    <t>NoPaymentEn</t>
+  </si>
+  <si>
+    <t>NoPaymentAr</t>
+  </si>
+  <si>
+    <t>No payments are found for this account</t>
+  </si>
+  <si>
+    <t>لا يوجد مدفوعات لهذا الحساب</t>
+  </si>
+  <si>
+    <t>AlternateManaged</t>
+  </si>
+  <si>
+    <t>Alternate Managed</t>
+  </si>
+  <si>
+    <t>TvsmobileTwo</t>
+  </si>
+  <si>
+    <t>Tvsmobiletwo Lastname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +349,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -366,12 +399,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Hyperlink 2" xfId="5"/>
@@ -673,15 +715,15 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -695,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,13 +762,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -734,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -742,7 +784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -750,7 +792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -758,7 +800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -766,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -774,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -782,7 +824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -790,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -811,13 +853,13 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -838,13 +880,13 @@
       <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -852,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -860,7 +902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -868,7 +910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -887,16 +929,16 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -904,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -912,7 +954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -920,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -928,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -936,7 +978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -944,7 +986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -952,7 +994,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -960,7 +1002,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -968,12 +1010,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -981,7 +1023,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -989,7 +1031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -997,7 +1039,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1005,7 +1047,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1013,7 +1055,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1021,7 +1063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1029,7 +1071,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1037,7 +1079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1045,7 +1087,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1053,7 +1095,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1061,7 +1103,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1069,7 +1111,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1077,7 +1119,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1095,17 +1137,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1121,7 +1163,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1136,19 +1178,79 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1164,7 +1266,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1172,7 +1274,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1180,7 +1282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1188,7 +1290,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1202,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1210,13 +1312,13 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1232,7 +1334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>